<commit_message>
Added the key values for vessel/voyage to the process
</commit_message>
<xml_diff>
--- a/Maersk/Test.xlsx
+++ b/Maersk/Test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\OneDrive - Blume Global\UiPath\OceanCarrierRPA\Maersk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\blume-proj\OceanCarrierRPA\Maersk\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -63,88 +63,88 @@
     <t>MAEU582369051</t>
   </si>
   <si>
+    <t>MAEU581991578</t>
+  </si>
+  <si>
+    <t>9075906332-01</t>
+  </si>
+  <si>
+    <t>922W</t>
+  </si>
+  <si>
+    <t>LEO C</t>
+  </si>
+  <si>
+    <t>MRKU0923491</t>
+  </si>
+  <si>
+    <t>DJMTYA4281416</t>
+  </si>
+  <si>
+    <t>SOVEREIGN MAERSK</t>
+  </si>
+  <si>
+    <t>MAEU4695834</t>
+  </si>
+  <si>
+    <t>MAEU583903133</t>
+  </si>
+  <si>
+    <t>DJPHXA4280956</t>
+  </si>
+  <si>
+    <t>MSC LAURENCE</t>
+  </si>
+  <si>
+    <t>MSKU8344306</t>
+  </si>
+  <si>
+    <t>MAEU582231406</t>
+  </si>
+  <si>
+    <t>9075906114-01</t>
+  </si>
+  <si>
+    <t>919W</t>
+  </si>
+  <si>
+    <t>MAERSK PITTSBURGH</t>
+  </si>
+  <si>
+    <t>MRKU6443798</t>
+  </si>
+  <si>
+    <t>MAEU581995129</t>
+  </si>
+  <si>
+    <t>MSC BREMEN</t>
+  </si>
+  <si>
+    <t>PONU1826841</t>
+  </si>
+  <si>
+    <t>MAEU582003720</t>
+  </si>
+  <si>
+    <t>T190072479</t>
+  </si>
+  <si>
+    <t>MAERSK CHICAGO</t>
+  </si>
+  <si>
+    <t>MRKU4147930</t>
+  </si>
+  <si>
+    <t>6702667F</t>
+  </si>
+  <si>
+    <t>PONU1581040</t>
+  </si>
+  <si>
+    <t>6702668F</t>
+  </si>
+  <si>
     <t>PONU1288242</t>
-  </si>
-  <si>
-    <t>6702668F</t>
-  </si>
-  <si>
-    <t>PONU1581040</t>
-  </si>
-  <si>
-    <t>6702667F</t>
-  </si>
-  <si>
-    <t>MRKU4147930</t>
-  </si>
-  <si>
-    <t>MAERSK CHICAGO</t>
-  </si>
-  <si>
-    <t>T190072479</t>
-  </si>
-  <si>
-    <t>MAEU582003720</t>
-  </si>
-  <si>
-    <t>PONU1826841</t>
-  </si>
-  <si>
-    <t>MSC BREMEN</t>
-  </si>
-  <si>
-    <t>922W</t>
-  </si>
-  <si>
-    <t>MAEU581995129</t>
-  </si>
-  <si>
-    <t>MRKU6443798</t>
-  </si>
-  <si>
-    <t>MAERSK PITTSBURGH</t>
-  </si>
-  <si>
-    <t>919W</t>
-  </si>
-  <si>
-    <t>9075906114-01</t>
-  </si>
-  <si>
-    <t>MAEU582231406</t>
-  </si>
-  <si>
-    <t>MSKU8344306</t>
-  </si>
-  <si>
-    <t>MSC LAURENCE</t>
-  </si>
-  <si>
-    <t>DJPHXA4280956</t>
-  </si>
-  <si>
-    <t>MAEU583903133</t>
-  </si>
-  <si>
-    <t>MAEU4695834</t>
-  </si>
-  <si>
-    <t>SOVEREIGN MAERSK</t>
-  </si>
-  <si>
-    <t>DJMTYA4281416</t>
-  </si>
-  <si>
-    <t>MRKU0923491</t>
-  </si>
-  <si>
-    <t>LEO C</t>
-  </si>
-  <si>
-    <t>9075906332-01</t>
-  </si>
-  <si>
-    <t>MAEU581991578</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:F21"/>
+      <selection activeCell="A4" sqref="A4:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,7 +529,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -538,7 +538,7 @@
         <v>923</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
@@ -546,7 +546,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -555,7 +555,7 @@
         <v>923</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -563,33 +563,33 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C6">
         <v>918</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>7250581131</v>
@@ -598,58 +598,58 @@
         <v>7250581131</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>921</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="E9">
         <v>7110243633</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>918</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="E10">
         <v>719778522</v>
@@ -660,19 +660,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>